<commit_message>
The Tuning Of Pre and Final Question and Answer Template With All Types Of Questions
</commit_message>
<xml_diff>
--- a/OperationalExcellence/Templates/ProductAssessment/FinalTestTemplate.xlsx
+++ b/OperationalExcellence/Templates/ProductAssessment/FinalTestTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simtuitive-Core\products\OperationalExcellence\Templates\ProductAssessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codebase-simtuitive-core-dev\product-templates\OperationalExcellence\Templates\ProductAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A549A2BB-4C11-48B4-82A7-A63B5454A18A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6173ED16-21AB-498E-8B20-2411B8A48DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5CB4F19B-C9F1-4F26-B1F4-4784C1ABDEB1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>No</t>
   </si>
@@ -58,6 +58,126 @@
   </si>
   <si>
     <t>Points</t>
+  </si>
+  <si>
+    <t>QnDescImage</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>NameQnImage-7</t>
+  </si>
+  <si>
+    <t>NameQnImage-8</t>
+  </si>
+  <si>
+    <t>NameQnImage-9</t>
+  </si>
+  <si>
+    <t>NameQnImage-10</t>
+  </si>
+  <si>
+    <t>NameQnImage-11</t>
+  </si>
+  <si>
+    <t>NameQnImage-12</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>IOWDF</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>TFWDF</t>
+  </si>
+  <si>
+    <t>DataFileName</t>
+  </si>
+  <si>
+    <t>DataFile7Name</t>
+  </si>
+  <si>
+    <t>DataFile8Name</t>
+  </si>
+  <si>
+    <t>DataFile9Name</t>
+  </si>
+  <si>
+    <t>DataFile10Name</t>
+  </si>
+  <si>
+    <t>DataFile11Name</t>
+  </si>
+  <si>
+    <t>DataFile12Name</t>
+  </si>
+  <si>
+    <t>Option3</t>
+  </si>
+  <si>
+    <t>Option4</t>
+  </si>
+  <si>
+    <t>Image17Name</t>
+  </si>
+  <si>
+    <t>Image18Name</t>
+  </si>
+  <si>
+    <t>Image19Name</t>
+  </si>
+  <si>
+    <t>Image20Name</t>
+  </si>
+  <si>
+    <t>Image21Name</t>
+  </si>
+  <si>
+    <t>Image22Name</t>
+  </si>
+  <si>
+    <t>Image23Name</t>
+  </si>
+  <si>
+    <t>Image24Name</t>
+  </si>
+  <si>
+    <t>Image25Name</t>
+  </si>
+  <si>
+    <t>Image26Name</t>
+  </si>
+  <si>
+    <t>Image27Name</t>
+  </si>
+  <si>
+    <t>Image28Name</t>
+  </si>
+  <si>
+    <t>Image29Name</t>
+  </si>
+  <si>
+    <t>Image30Name</t>
+  </si>
+  <si>
+    <t>Image31Name</t>
+  </si>
+  <si>
+    <t>Image32Name</t>
   </si>
 </sst>
 </file>
@@ -416,21 +536,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E761E6-F95A-4BF3-81F7-E1827973A4E2}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,25 +561,451 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>43</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>51</v>
+      </c>
+      <c r="H8">
+        <v>52</v>
+      </c>
+      <c r="I8">
+        <v>53</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>61</v>
+      </c>
+      <c r="H9">
+        <v>62</v>
+      </c>
+      <c r="I9">
+        <v>63</v>
+      </c>
+      <c r="J9">
+        <v>62</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>